<commit_message>
aaron vs kai wb update
</commit_message>
<xml_diff>
--- a/kai/kai-warband.xlsx
+++ b/kai/kai-warband.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6372F31-F427-4AE1-8DFB-E398216960CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE761DA-210A-40EF-A9CF-F8F1DD545ACA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,6 +646,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -658,7 +659,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1067,7 +1067,7 @@
   <dimension ref="A2:AA115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1114,7 +1114,7 @@
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="19">
-        <v>43450</v>
+        <v>43464</v>
       </c>
       <c r="G2" t="s">
         <v>97</v>
@@ -1287,7 +1287,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="59" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
@@ -1317,7 +1317,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="58"/>
+      <c r="A13" s="59"/>
       <c r="B13" t="s">
         <v>54</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="58"/>
+      <c r="A14" s="59"/>
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
@@ -1397,7 +1397,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="58"/>
+      <c r="A16" s="59"/>
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="58"/>
+      <c r="A17" s="59"/>
       <c r="B17" t="s">
         <v>57</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="58"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="5" t="s">
         <v>56</v>
       </c>
@@ -1511,30 +1511,30 @@
         <v>12</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="H20" s="59" t="s">
+      <c r="H20" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59" t="s">
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
@@ -1588,7 +1588,7 @@
       <c r="R22" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="S22" s="62" t="s">
+      <c r="S22" s="58" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2822,11 +2822,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:14" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="31"/>
@@ -2839,21 +2839,21 @@
       <c r="D4" s="31"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61" t="s">
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="K5" s="59" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="K5" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="L5" s="59"/>
+      <c r="L5" s="60"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>

</xml_diff>